<commit_message>
Matrix tutorial test - finalized
</commit_message>
<xml_diff>
--- a/profilePresntaion/myUtils/instructions.xlsx
+++ b/profilePresntaion/myUtils/instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\WebExp\WebExperiment\profilePresntaion\myUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFD5E19-F06A-4CC4-A4A9-89CE2887F5F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6320B8C6-B0E1-4124-9E92-EFD3CEBFF426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>phase</t>
   </si>
@@ -66,9 +66,6 @@
     <t>בזמו שמוצג</t>
   </si>
   <si>
-    <t>מטריצות בתשלומים יש {} וגם יש שני {}</t>
-  </si>
-  <si>
     <t>לפני הצגת  הפרופיל</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
     <t>text_he</t>
   </si>
   <si>
-    <t>שלב שני</t>
-  </si>
-  <si>
-    <t>שלב שלישי</t>
-  </si>
-  <si>
     <t>off_order_place</t>
   </si>
   <si>
@@ -103,6 +94,18 @@
   </si>
   <si>
     <t>במידה ואת.ה תבחר.י - {} - והאדם השני יבחר - {}, כמה האדם השני יקבל?</t>
+  </si>
+  <si>
+    <t>במהלך הניסוי יוצגו לך פרופילים של אנשים שונים. לאחר שתתבונן בפרופיל של כל אדם, תשחק מול משחק הקשור לסיואציה בו אתם כביכול נפגשים. המשחק מתאר שתי בחירות אפשריות שלך  ושתי בחירות אפשריות של האחר. עבור כל שילוב של שתי בחירות ישנה תוצאה אשר מיוצגת במספר, תוצאה עבורך ותוצאה עבור האחר. לחץ על הכפתור Ready to play על מנת להתבונן במשחק</t>
+  </si>
+  <si>
+    <t>יפה מאוד! כאשר אתה לוחץ על אחת השורות, זה אומר שבחרת באפשרות הזו. כמה שתקבל תלוי במה יבחר השחקן השני. בזמן שאתה מבצע את בחירתך אינך יכול לראות מה השחקן השני בחר, אך גם כשאר השחקן השני בוחר, אתה לא יכול לראות את הבחירה שלו. תוצאות המשחק יקבעו רק לאחר מכן. בוא נמשיך בלמידה - לחץ עכשיו על האופציה העליונה.</t>
+  </si>
+  <si>
+    <t>מעולה! כעת, ענה על השאלות שמופיעות מטה. בכל שאלה תצטרך לומר כמה אתה או השחק האחר יקבלו עבור שילוב מסוים של שתי אפשרויות, הבחירה שלך והבחירה של האחר.</t>
+  </si>
+  <si>
+    <t>במשחק זה אתה יכול לבחור בין {} , לבין {} וכך גם האדם השני. כל אחד מכם בוחר לפי ראות עיניו, ומתוך הניסיון להגיע לתוצאה הטובה ביותר עבורו. אתה יכול לבחור או בשורה הראשונה ({}) או בשורה השניה ({}). כך גם השחקן השני, אל שהוא יכול לבחור בין הטור הימני לשמאלי. בכל צירוף של שתי בחירות רשום כמה אתה תקבל וכמה האחר. התוצאה שלך רשומה תמיד מצד שמאל. לצורך בדיקת הבנה - בחר כעת את השורה התחונה - {}.</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,10 +449,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -460,7 +463,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -471,7 +474,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -482,7 +485,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -493,7 +496,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -501,10 +504,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -512,10 +515,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,10 +526,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -534,54 +537,65 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes before changing computer
</commit_message>
<xml_diff>
--- a/profilePresntaion/myUtils/instructions.xlsx
+++ b/profilePresntaion/myUtils/instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\WebExp\WebExperiment\profilePresntaion\myUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6320B8C6-B0E1-4124-9E92-EFD3CEBFF426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7298288-7070-46FB-9597-5D17E3196100}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>phase</t>
   </si>
@@ -54,12 +54,6 @@
     <t>end</t>
   </si>
   <si>
-    <t>זהו טופס הסכמה</t>
-  </si>
-  <si>
-    <t>לפני פרופיל</t>
-  </si>
-  <si>
     <t>לפני שמתחילים</t>
   </si>
   <si>
@@ -106,6 +100,43 @@
   </si>
   <si>
     <t>במשחק זה אתה יכול לבחור בין {} , לבין {} וכך גם האדם השני. כל אחד מכם בוחר לפי ראות עיניו, ומתוך הניסיון להגיע לתוצאה הטובה ביותר עבורו. אתה יכול לבחור או בשורה הראשונה ({}) או בשורה השניה ({}). כך גם השחקן השני, אל שהוא יכול לבחור בין הטור הימני לשמאלי. בכל צירוף של שתי בחירות רשום כמה אתה תקבל וכמה האחר. התוצאה שלך רשומה תמיד מצד שמאל. לצורך בדיקת הבנה - בחר כעת את השורה התחונה - {}.</t>
+  </si>
+  <si>
+    <t>Identification Task</t>
+  </si>
+  <si>
+    <t>השאלון שעליו את/ה עומד/ת לענות הוא חלק ממחקר פסיכולוגי שבוחן את הרגשות והחוויות בחיי היום יום.
+את/ה חופשי/ה לחלוטין להחליט האם את/ה מעוניין/ת להשתתף במחקר.
+במידה ותחליט/ילהשתתף, את/ה רשאי/ת להחליט להפסיק לגמרי את השתתפותך במחקר בכל שלב.
+נדגיש גם כי לא תתבקש/י למסור פרטים מזהים בשאלון זה, על כן תשובותיך ישמרו באופן אנונימי.
+ככל הידוע השתתפות במחקר אינה כרוכה בסיכונים כלשהם.
+אם ברצונך לשמור עותק מדף זה, ניתן להדפיס את העמוד כעת.</t>
+  </si>
+  <si>
+    <t>הדירוגים שסיפקת יוצרים פרופיל אישי שלך וכך גם דירוגיהם של המשתתפים הנוספים בניסוי.
+בחלק הזה של הניסוי יוצגו בפניך שני פרופילים בו זמנית, אחד בצד ימין והשני בצד שמאל. אחד מהפרופילים האלו הוא שלך, כלומר מתאר את המאפיין אותם דירגת כעת, והשני הוא של משתתף אחר. 
+המטלה שלך היא להתבונן היטב בשני הפרופילים, ולזהות מה הוא הפרופיל שלך.</t>
+  </si>
+  <si>
+    <t>לאחר כ-30 שניות יופיע מתחת לכל אחד מהפרופילים כפתור שעליו כתוב "זה הפרופיל שלי". אם תאה חושב שפרופיל ימין הוא הפרופיל שלך בחר בכפתור הימני, זה שיופיע מתחת לפרופיל הימני. לחילופין, בחר בכפתור השמאלי אם אתה חושב שהפרופיל שלך הוא השמאלי. 
+קח את כל הזמן הדרוש כדי להגיע להחלטה הנכונה, גם אם כבר עבור 30 שניות.
+כאשר תלחץ על הכפתור יתחלפו הפרופילים ותצטרך לבחור שוב.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">כעת תבצע מטלה מאוד דומה למטלה שביצע קודם, אלא שהשינוי המרכזי כאן הוא שלא תצטרף להמתין 30 שניות, אלא תצטרך להגיב כמה שיותר מהר. כלומר, ברגע שיופיעו שני הפרופילים, באופן אוטומטי גם יופיעו שני הכפתורים. המטרה שלך תהיה להחליט כמה שיותר מהר באיזה צד מופיע הפרופיל שלך וללחוץ על הכפתור שנמצא בצד המתאים.
+שים לב, עליך לדייק ויחד עם זאת להגיב במהירות. </t>
+  </si>
+  <si>
+    <t>Pre Identification Task</t>
+  </si>
+  <si>
+    <t>preQuickPhase</t>
+  </si>
+  <si>
+    <t>בחלק זה של הניסוי זה תתבקש\י לענות על מספר שאלות.
+כל שאלה תעסוק במאפיין שונה שלך, למשל תכונות אופי ואישיות, תחביבים וכדומה.
+התשובה לשאלות תיעשה על ידי הזזה של סמן הנמצא בין שני קצוות, כך שהמקום אותו תבחר\י יתאר אותך בצורה הטובה והמדויקת ביותר.
+ לאחר בחירת מיקום הסמן, לחצ\י על הכפתור &lt;בחר והמשך&gt; אשר יופיע בתחתית המסך.</t>
   </si>
 </sst>
 </file>
@@ -149,9 +180,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,16 +466,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" customWidth="1"/>
+    <col min="2" max="2" width="83.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -449,21 +483,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -471,21 +505,21 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -493,43 +527,43 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -537,10 +571,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,10 +582,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -562,40 +596,73 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>